<commit_message>
based format on first valid sheet
</commit_message>
<xml_diff>
--- a/tests/OSPSuite.R.Tests/Data/BookStrings.xlsx
+++ b/tests/OSPSuite.R.Tests/Data/BookStrings.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AbdelRodriguez\Documents\GitHub\OSPSuite.Core\tests\OSPSuite.R.Tests\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00BED545-EFCC-4074-AE51-4B47C29B6E27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7B90724-B77B-4FEF-9027-09357A6955AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{6AF95343-47B6-4DBD-AB5D-C2CA9D4DA7C3}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="4">
   <si>
     <t>Time [h]</t>
   </si>
@@ -1236,14 +1236,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0725EA5A-171B-46B1-BCD4-B0DC7D3FEEF2}">
-  <dimension ref="A1"/>
+  <dimension ref="A2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <sheetData>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
@@ -1254,7 +1260,7 @@
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="A1:C9"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>